<commit_message>
dataproc and predictive progress
</commit_message>
<xml_diff>
--- a/BTC_Transaction_LIVE.xlsx
+++ b/BTC_Transaction_LIVE.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>17.38577946768061</v>
+        <v>16.83409812409812</v>
       </c>
       <c r="C2" t="n">
-        <v>317394649438</v>
+        <v>114911569152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched to new branch
</commit_message>
<xml_diff>
--- a/BTC_Transaction_LIVE.xlsx
+++ b/BTC_Transaction_LIVE.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>83.80255797359975</v>
+        <v>35.77720375888149</v>
       </c>
       <c r="C2" t="n">
-        <v>1532479293066</v>
+        <v>277814641172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>